<commit_message>
feat: Plotting results and RSM method
</commit_message>
<xml_diff>
--- a/RankingMethods/dane.xlsx
+++ b/RankingMethods/dane.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konrad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\StudiaMagisterskie\SemestrII\Optymalizacja wielokryterialna\OptymalizacjaWielokryterialna\RankingMethods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15185BE-EE6C-4D2E-BEE2-333B7DF1ADF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D982F5E-7788-446C-BE2F-8EE057881927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E3F5E22A-33F6-4C0E-8A90-E2FEEE9C71BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E3F5E22A-33F6-4C0E-8A90-E2FEEE9C71BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="123">
   <si>
     <t>Marża [%]</t>
   </si>
@@ -4461,1399 +4461,587 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB0CF73-CF8D-44C7-ABDF-24FDD6566452}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:H53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="B1" s="1">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1.84</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>2.04</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2.08</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="B9" s="1">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>2.09</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>1.96</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>1.94</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>2.04</v>
+      </c>
+      <c r="B23" s="1">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>1.97</v>
+      </c>
+      <c r="B24" s="1">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B26" s="1">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="B27" s="1">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="B29" s="1">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="B30" s="1">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>2.33</v>
+      </c>
+      <c r="B31" s="1">
+        <v>20</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="B32" s="1">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B33" s="1">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B34" s="1">
+        <v>20</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B35" s="1">
+        <v>20</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1">
+        <v>20</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="B37" s="1">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.65</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4.24</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2066</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5.28</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2183</v>
-      </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.84</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5.09</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2214</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>2.39</v>
+      </c>
+      <c r="B38" s="1">
+        <v>20</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
         <v>1.85</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5.16</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2255</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B39" s="1">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="B40" s="1">
+        <v>20</v>
+      </c>
+      <c r="C40" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="B41" s="1">
+        <v>20</v>
+      </c>
+      <c r="C41" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1">
+        <v>20</v>
+      </c>
+      <c r="C42" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>2.09</v>
+      </c>
+      <c r="B43" s="1">
+        <v>20</v>
+      </c>
+      <c r="C43" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B44" s="1">
+        <v>20</v>
+      </c>
+      <c r="C44" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="B45" s="1">
+        <v>20</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>1.96</v>
+      </c>
+      <c r="B46" s="1">
+        <v>20</v>
+      </c>
+      <c r="C46" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>2.29</v>
+      </c>
+      <c r="B47" s="1">
+        <v>20</v>
+      </c>
+      <c r="C47" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>2.39</v>
+      </c>
+      <c r="B48" s="1">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>2.29</v>
+      </c>
+      <c r="B49" s="1">
+        <v>20</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B50" s="1">
+        <v>20</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
         <v>2.04</v>
       </c>
-      <c r="D6" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5.28</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2264</v>
-      </c>
-      <c r="G6" s="1">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5.04</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2274</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5.42</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2314</v>
-      </c>
-      <c r="G8" s="1">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.08</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5.74</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2345</v>
-      </c>
-      <c r="G9" s="1">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.19</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5.83</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2369</v>
-      </c>
-      <c r="G10" s="1">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>6.02</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2482</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.09</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>4.8</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2264</v>
-      </c>
-      <c r="G12" s="1">
-        <v>41</v>
-      </c>
-      <c r="H12" s="1">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="E13" s="1">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2291</v>
-      </c>
-      <c r="G13" s="1">
-        <v>41</v>
-      </c>
-      <c r="H13" s="1">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2241</v>
-      </c>
-      <c r="G14" s="1">
-        <v>41</v>
-      </c>
-      <c r="H14" s="1">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>4.75</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2255</v>
-      </c>
-      <c r="G15" s="1">
-        <v>41</v>
-      </c>
-      <c r="H15" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="E16" s="1">
-        <v>5.65</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2347</v>
-      </c>
-      <c r="G16" s="1">
-        <v>41</v>
-      </c>
-      <c r="H16" s="1">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>4.8</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2264</v>
-      </c>
-      <c r="G17" s="1">
-        <v>41</v>
-      </c>
-      <c r="H17" s="1">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>5.44</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2408</v>
-      </c>
-      <c r="G18" s="1">
-        <v>41</v>
-      </c>
-      <c r="H18" s="1">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1.96</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>5.92</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2371</v>
-      </c>
-      <c r="G19" s="1">
-        <v>41</v>
-      </c>
-      <c r="H19" s="1">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1.95</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5.58</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2371</v>
-      </c>
-      <c r="G20" s="1">
-        <v>41</v>
-      </c>
-      <c r="H20" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1.94</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2</v>
-      </c>
-      <c r="E21" s="1">
-        <v>6.08</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2501</v>
-      </c>
-      <c r="G21" s="1">
-        <v>41</v>
-      </c>
-      <c r="H21" s="1">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1">
-        <v>5.52</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2382</v>
-      </c>
-      <c r="G22" s="1">
-        <v>41</v>
-      </c>
-      <c r="H22" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1">
-        <v>4</v>
-      </c>
-      <c r="E23" s="1">
-        <v>5.05</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2324.09</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2.04</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="E24" s="1">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2135.38</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.97</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="E25" s="1">
-        <v>4.08</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2113.39</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2</v>
-      </c>
-      <c r="D26" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="E26" s="1">
-        <v>4.05</v>
-      </c>
-      <c r="F26" s="1">
-        <v>2106.04</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>3.88</v>
-      </c>
-      <c r="F27" s="1">
-        <v>2070.5</v>
-      </c>
-      <c r="G27" s="1">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="E28" s="1">
-        <v>3.82</v>
-      </c>
-      <c r="F28" s="1">
-        <v>2058.75</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
-        <v>3.79</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2052.17</v>
-      </c>
-      <c r="G29" s="1">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1.95</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="E30" s="1">
-        <v>3.72</v>
-      </c>
-      <c r="F30" s="1">
-        <v>2036.89</v>
-      </c>
-      <c r="G30" s="1">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>3.68</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2020.33</v>
-      </c>
-      <c r="G31" s="1">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2.33</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="B51" s="1">
+        <v>20</v>
+      </c>
+      <c r="C51" s="1">
         <v>2.8</v>
       </c>
-      <c r="F32" s="1">
-        <v>1578.36</v>
-      </c>
-      <c r="G32" s="1">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="E33" s="1">
-        <v>3.7</v>
-      </c>
-      <c r="F33" s="1">
-        <v>1755.09</v>
-      </c>
-      <c r="G33" s="1">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="E34" s="1">
-        <v>2.54</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1762.94</v>
-      </c>
-      <c r="G34" s="1">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="1">
-        <v>2</v>
-      </c>
-      <c r="D35" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="E35" s="1">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1797.92</v>
-      </c>
-      <c r="G35" s="1">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="D36" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="E36" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="F36" s="1">
-        <v>1863.53</v>
-      </c>
-      <c r="G36" s="1">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="1">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="E37" s="1">
-        <v>5.01</v>
-      </c>
-      <c r="F37" s="1">
-        <v>2126.63</v>
-      </c>
-      <c r="G37" s="1">
-        <v>20</v>
-      </c>
-      <c r="H37" s="1">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1.85</v>
-      </c>
-      <c r="D38" s="1">
-        <v>0</v>
-      </c>
-      <c r="E38" s="1">
-        <v>4.62</v>
-      </c>
-      <c r="F38" s="1">
-        <v>2216.52</v>
-      </c>
-      <c r="G38" s="1">
-        <v>20</v>
-      </c>
-      <c r="H38" s="1">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>2.39</v>
+      </c>
+      <c r="B52" s="1">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="1">
-        <v>2.39</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2</v>
-      </c>
-      <c r="E39" s="1">
-        <v>5.38</v>
-      </c>
-      <c r="F39" s="1">
-        <v>2340.69</v>
-      </c>
-      <c r="G39" s="1">
-        <v>20</v>
-      </c>
-      <c r="H39" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1.85</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1">
-        <v>4.62</v>
-      </c>
-      <c r="F40" s="1">
-        <v>2217</v>
-      </c>
-      <c r="G40" s="1">
-        <v>20</v>
-      </c>
-      <c r="H40" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="E41" s="1">
-        <v>4.7699999999999996</v>
-      </c>
-      <c r="F41" s="1">
-        <v>2226</v>
-      </c>
-      <c r="G41" s="1">
-        <v>20</v>
-      </c>
-      <c r="H41" s="1">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="F42" s="1">
-        <v>2226</v>
-      </c>
-      <c r="G42" s="1">
-        <v>20</v>
-      </c>
-      <c r="H42" s="1">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>103</v>
-      </c>
-      <c r="B43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="1">
-        <v>2</v>
-      </c>
-      <c r="D43" s="1">
-        <v>0</v>
-      </c>
-      <c r="E43" s="1">
-        <v>4.7699999999999996</v>
-      </c>
-      <c r="F43" s="1">
-        <v>2251</v>
-      </c>
-      <c r="G43" s="1">
-        <v>20</v>
-      </c>
-      <c r="H43" s="1">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="1">
-        <v>2.09</v>
-      </c>
-      <c r="D44" s="1">
-        <v>0</v>
-      </c>
-      <c r="E44" s="1">
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="F44" s="1">
-        <v>2271</v>
-      </c>
-      <c r="G44" s="1">
-        <v>20</v>
-      </c>
-      <c r="H44" s="1">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>105</v>
-      </c>
-      <c r="B45" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="D45" s="1">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1">
-        <v>4.87</v>
-      </c>
-      <c r="F45" s="1">
-        <v>2274</v>
-      </c>
-      <c r="G45" s="1">
-        <v>20</v>
-      </c>
-      <c r="H45" s="1">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="E46" s="1">
-        <v>5.07</v>
-      </c>
-      <c r="F46" s="1">
-        <v>2299</v>
-      </c>
-      <c r="G46" s="1">
-        <v>20</v>
-      </c>
-      <c r="H46" s="1">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1.96</v>
-      </c>
-      <c r="D47" s="1">
-        <v>0</v>
-      </c>
-      <c r="E47" s="1">
-        <v>5.04</v>
-      </c>
-      <c r="F47" s="1">
-        <v>2315</v>
-      </c>
-      <c r="G47" s="1">
-        <v>20</v>
-      </c>
-      <c r="H47" s="1">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>108</v>
-      </c>
-      <c r="B48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="D48" s="1">
-        <v>2</v>
-      </c>
-      <c r="E48" s="1">
-        <v>5.33</v>
-      </c>
-      <c r="F48" s="1">
-        <v>2317</v>
-      </c>
-      <c r="G48" s="1">
-        <v>20</v>
-      </c>
-      <c r="H48" s="1">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B49" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="1">
-        <v>2.39</v>
-      </c>
-      <c r="D49" s="1">
-        <v>2</v>
-      </c>
-      <c r="E49" s="1">
-        <v>5.37</v>
-      </c>
-      <c r="F49" s="1">
-        <v>2341</v>
-      </c>
-      <c r="G49" s="1">
-        <v>20</v>
-      </c>
-      <c r="H49" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>110</v>
-      </c>
-      <c r="B50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="D50" s="1">
-        <v>2</v>
-      </c>
-      <c r="E50" s="1">
-        <v>5.61</v>
-      </c>
-      <c r="F50" s="1">
-        <v>2392</v>
-      </c>
-      <c r="G50" s="1">
-        <v>20</v>
-      </c>
-      <c r="H50" s="1">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="D51" s="1">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1">
-        <v>4.7300000000000004</v>
-      </c>
-      <c r="F51" s="1">
-        <v>2275.87</v>
-      </c>
-      <c r="G51" s="1">
-        <v>20</v>
-      </c>
-      <c r="H51" s="1">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="1">
-        <v>2.04</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="E52" s="1">
-        <v>4.9800000000000004</v>
-      </c>
-      <c r="F52" s="1">
-        <v>2307.12</v>
-      </c>
-      <c r="G52" s="1">
-        <v>20</v>
-      </c>
-      <c r="H52" s="1">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="1">
-        <v>2.39</v>
-      </c>
-      <c r="D53" s="1">
-        <v>2</v>
-      </c>
-      <c r="E53" s="1">
-        <v>5.35</v>
-      </c>
-      <c r="F53" s="1">
-        <v>2389.88</v>
-      </c>
-      <c r="G53" s="1">
-        <v>20</v>
-      </c>
-      <c r="H53" s="1">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G53">
-    <sortCondition ref="E1:E53"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5862,7 +5050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49853C66-9C62-4FF8-97FB-D16C416F8D4C}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>